<commit_message>
update database + fix search
</commit_message>
<xml_diff>
--- a/docs/temp/Tasksheet.xlsx
+++ b/docs/temp/Tasksheet.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FPT\CarRentalPortal\docs\temp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="1665" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -16,7 +21,7 @@
     <definedName name="_Toc448316378" localSheetId="0">Sheet1!$C$64</definedName>
     <definedName name="_Toc448316400" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +36,7 @@
     <author>phuong</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0">
+    <comment ref="C16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0">
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -439,14 +444,14 @@
     <t>Provider functions</t>
   </si>
   <si>
-    <t>Main day</t>
+    <t>Man-day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -685,6 +690,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -699,9 +707,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -758,6 +763,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -805,7 +813,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -840,7 +848,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1049,16 +1057,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
     <col min="3" max="3" width="59.85546875" customWidth="1"/>
@@ -1069,7 +1077,7 @@
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1095,11 +1103,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="25">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1115,9 +1123,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75">
-      <c r="A3" s="25"/>
-      <c r="B3" s="24"/>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
@@ -1131,9 +1139,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75">
-      <c r="A4" s="25"/>
-      <c r="B4" s="24"/>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
@@ -1147,9 +1155,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75">
-      <c r="A5" s="25"/>
-      <c r="B5" s="24"/>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
@@ -1163,9 +1171,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75">
-      <c r="A6" s="25"/>
-      <c r="B6" s="24"/>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1181,9 +1189,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75">
-      <c r="A7" s="25"/>
-      <c r="B7" s="24"/>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
@@ -1197,9 +1205,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75">
-      <c r="A8" s="25"/>
-      <c r="B8" s="24"/>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
@@ -1213,9 +1221,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75">
-      <c r="A9" s="25"/>
-      <c r="B9" s="24"/>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
@@ -1229,11 +1237,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75">
-      <c r="A10" s="25">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="26">
         <v>2</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1249,9 +1257,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75">
-      <c r="A11" s="25"/>
-      <c r="B11" s="24"/>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1265,9 +1273,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75">
-      <c r="A12" s="25"/>
-      <c r="B12" s="24"/>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1281,9 +1289,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75">
-      <c r="A13" s="25"/>
-      <c r="B13" s="24"/>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1297,9 +1305,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75">
-      <c r="A14" s="25"/>
-      <c r="B14" s="24"/>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1313,11 +1321,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="25">
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
         <v>3</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -1333,9 +1341,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75">
-      <c r="A16" s="25"/>
-      <c r="B16" s="24"/>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1345,9 +1353,9 @@
       <c r="G16" s="19"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75">
-      <c r="A17" s="25"/>
-      <c r="B17" s="24"/>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="7" t="s">
         <v>27</v>
       </c>
@@ -1361,9 +1369,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75">
-      <c r="A18" s="25"/>
-      <c r="B18" s="24"/>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="7" t="s">
         <v>26</v>
       </c>
@@ -1377,9 +1385,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75">
-      <c r="A19" s="25"/>
-      <c r="B19" s="24"/>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="8" t="s">
         <v>28</v>
       </c>
@@ -1389,9 +1397,9 @@
       <c r="G19" s="19"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75">
-      <c r="A20" s="25"/>
-      <c r="B20" s="24"/>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="9" t="s">
         <v>54</v>
       </c>
@@ -1405,9 +1413,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75">
-      <c r="A21" s="25"/>
-      <c r="B21" s="24"/>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="9" t="s">
         <v>55</v>
       </c>
@@ -1421,9 +1429,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75">
-      <c r="A22" s="25"/>
-      <c r="B22" s="24"/>
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="9" t="s">
         <v>56</v>
       </c>
@@ -1437,9 +1445,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75">
-      <c r="A23" s="25"/>
-      <c r="B23" s="24"/>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="9" t="s">
         <v>57</v>
       </c>
@@ -1453,9 +1461,9 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75">
-      <c r="A24" s="25"/>
-      <c r="B24" s="24"/>
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="9" t="s">
         <v>58</v>
       </c>
@@ -1468,9 +1476,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75">
-      <c r="A25" s="25"/>
-      <c r="B25" s="24"/>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="9" t="s">
         <v>59</v>
       </c>
@@ -1484,9 +1492,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75">
-      <c r="A26" s="25"/>
-      <c r="B26" s="24"/>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="9" t="s">
         <v>60</v>
       </c>
@@ -1500,9 +1508,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75">
-      <c r="A27" s="25"/>
-      <c r="B27" s="24"/>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="25"/>
       <c r="C27" s="9" t="s">
         <v>61</v>
       </c>
@@ -1516,9 +1524,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="25"/>
-      <c r="B28" s="24"/>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="9" t="s">
         <v>62</v>
       </c>
@@ -1531,9 +1539,9 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75">
-      <c r="A29" s="25"/>
-      <c r="B29" s="24"/>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" s="25"/>
       <c r="C29" s="15" t="s">
         <v>63</v>
       </c>
@@ -1547,9 +1555,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75">
-      <c r="A30" s="25"/>
-      <c r="B30" s="24"/>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="15" t="s">
         <v>64</v>
       </c>
@@ -1563,9 +1571,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75">
-      <c r="A31" s="25"/>
-      <c r="B31" s="24"/>
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="15" t="s">
         <v>65</v>
       </c>
@@ -1579,9 +1587,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75">
-      <c r="A32" s="25"/>
-      <c r="B32" s="24"/>
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
+      <c r="B32" s="25"/>
       <c r="C32" s="15" t="s">
         <v>66</v>
       </c>
@@ -1595,9 +1603,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75">
-      <c r="A33" s="25"/>
-      <c r="B33" s="24"/>
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="15" t="s">
         <v>67</v>
       </c>
@@ -1611,9 +1619,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.75">
-      <c r="A34" s="25"/>
-      <c r="B34" s="24"/>
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="26"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="15" t="s">
         <v>68</v>
       </c>
@@ -1627,9 +1635,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75">
-      <c r="A35" s="25"/>
-      <c r="B35" s="24"/>
+    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="25"/>
       <c r="C35" s="15" t="s">
         <v>69</v>
       </c>
@@ -1643,9 +1651,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75">
-      <c r="A36" s="25"/>
-      <c r="B36" s="24"/>
+    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="15" t="s">
         <v>70</v>
       </c>
@@ -1659,9 +1667,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75">
-      <c r="A37" s="25"/>
-      <c r="B37" s="24"/>
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="25"/>
       <c r="C37" s="9" t="s">
         <v>71</v>
       </c>
@@ -1675,9 +1683,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.75">
-      <c r="A38" s="25"/>
-      <c r="B38" s="24"/>
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="26"/>
+      <c r="B38" s="25"/>
       <c r="C38" s="9" t="s">
         <v>72</v>
       </c>
@@ -1691,9 +1699,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.75">
-      <c r="A39" s="25"/>
-      <c r="B39" s="24"/>
+    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="15" t="s">
         <v>73</v>
       </c>
@@ -1707,9 +1715,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.75">
-      <c r="A40" s="25"/>
-      <c r="B40" s="24"/>
+    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="26"/>
+      <c r="B40" s="25"/>
       <c r="C40" s="15" t="s">
         <v>74</v>
       </c>
@@ -1723,9 +1731,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75">
-      <c r="A41" s="25"/>
-      <c r="B41" s="24"/>
+    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="26"/>
+      <c r="B41" s="25"/>
       <c r="C41" s="9" t="s">
         <v>75</v>
       </c>
@@ -1739,9 +1747,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.75">
-      <c r="A42" s="25"/>
-      <c r="B42" s="24"/>
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="26"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="9" t="s">
         <v>76</v>
       </c>
@@ -1755,9 +1763,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75">
-      <c r="A43" s="25"/>
-      <c r="B43" s="24"/>
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="26"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="9" t="s">
         <v>77</v>
       </c>
@@ -1771,9 +1779,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75">
-      <c r="A44" s="25"/>
-      <c r="B44" s="24"/>
+    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="26"/>
+      <c r="B44" s="25"/>
       <c r="C44" s="9" t="s">
         <v>78</v>
       </c>
@@ -1787,9 +1795,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.75">
-      <c r="A45" s="25"/>
-      <c r="B45" s="24"/>
+    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="26"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="9" t="s">
         <v>79</v>
       </c>
@@ -1803,9 +1811,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15.75">
-      <c r="A46" s="25"/>
-      <c r="B46" s="24"/>
+    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="26"/>
+      <c r="B46" s="25"/>
       <c r="C46" s="9" t="s">
         <v>80</v>
       </c>
@@ -1819,9 +1827,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.75">
-      <c r="A47" s="25"/>
-      <c r="B47" s="24"/>
+    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="26"/>
+      <c r="B47" s="25"/>
       <c r="C47" s="9" t="s">
         <v>81</v>
       </c>
@@ -1835,9 +1843,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.75">
-      <c r="A48" s="25"/>
-      <c r="B48" s="24"/>
+    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="26"/>
+      <c r="B48" s="25"/>
       <c r="C48" s="9" t="s">
         <v>82</v>
       </c>
@@ -1851,9 +1859,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15.75">
-      <c r="A49" s="25"/>
-      <c r="B49" s="24"/>
+    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="26"/>
+      <c r="B49" s="25"/>
       <c r="C49" s="9" t="s">
         <v>83</v>
       </c>
@@ -1867,9 +1875,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75">
-      <c r="A50" s="25"/>
-      <c r="B50" s="24"/>
+    <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="26"/>
+      <c r="B50" s="25"/>
       <c r="C50" s="9" t="s">
         <v>84</v>
       </c>
@@ -1883,9 +1891,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75">
-      <c r="A51" s="25"/>
-      <c r="B51" s="24"/>
+    <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="26"/>
+      <c r="B51" s="25"/>
       <c r="C51" s="9" t="s">
         <v>85</v>
       </c>
@@ -1899,9 +1907,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15.75">
-      <c r="A52" s="25"/>
-      <c r="B52" s="24"/>
+    <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="26"/>
+      <c r="B52" s="25"/>
       <c r="C52" s="9" t="s">
         <v>86</v>
       </c>
@@ -1915,9 +1923,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15.75">
-      <c r="A53" s="25"/>
-      <c r="B53" s="24"/>
+    <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="26"/>
+      <c r="B53" s="25"/>
       <c r="C53" s="9" t="s">
         <v>87</v>
       </c>
@@ -1931,9 +1939,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="15.75">
-      <c r="A54" s="25"/>
-      <c r="B54" s="24"/>
+    <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="26"/>
+      <c r="B54" s="25"/>
       <c r="C54" s="9" t="s">
         <v>88</v>
       </c>
@@ -1947,9 +1955,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75">
-      <c r="A55" s="25"/>
-      <c r="B55" s="24"/>
+    <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="26"/>
+      <c r="B55" s="25"/>
       <c r="C55" s="9" t="s">
         <v>89</v>
       </c>
@@ -1963,9 +1971,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75">
-      <c r="A56" s="25"/>
-      <c r="B56" s="24"/>
+    <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="26"/>
+      <c r="B56" s="25"/>
       <c r="C56" s="9" t="s">
         <v>90</v>
       </c>
@@ -1979,9 +1987,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15.75">
-      <c r="A57" s="25"/>
-      <c r="B57" s="24"/>
+    <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="26"/>
+      <c r="B57" s="25"/>
       <c r="C57" s="9" t="s">
         <v>91</v>
       </c>
@@ -1995,9 +2003,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15.75">
-      <c r="A58" s="25"/>
-      <c r="B58" s="24"/>
+    <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="26"/>
+      <c r="B58" s="25"/>
       <c r="C58" s="9" t="s">
         <v>94</v>
       </c>
@@ -2011,9 +2019,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15.75">
-      <c r="A59" s="25"/>
-      <c r="B59" s="24"/>
+    <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="26"/>
+      <c r="B59" s="25"/>
       <c r="C59" s="9" t="s">
         <v>92</v>
       </c>
@@ -2027,9 +2035,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="15.75">
-      <c r="A60" s="25"/>
-      <c r="B60" s="24"/>
+    <row r="60" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="26"/>
+      <c r="B60" s="25"/>
       <c r="C60" s="9" t="s">
         <v>93</v>
       </c>
@@ -2043,9 +2051,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15.75">
-      <c r="A61" s="25"/>
-      <c r="B61" s="24"/>
+    <row r="61" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="26"/>
+      <c r="B61" s="25"/>
       <c r="C61" s="9" t="s">
         <v>95</v>
       </c>
@@ -2059,9 +2067,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75">
-      <c r="A62" s="25"/>
-      <c r="B62" s="24"/>
+    <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="26"/>
+      <c r="B62" s="25"/>
       <c r="C62" s="9" t="s">
         <v>96</v>
       </c>
@@ -2075,9 +2083,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15.75">
-      <c r="A63" s="25"/>
-      <c r="B63" s="24"/>
+    <row r="63" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="26"/>
+      <c r="B63" s="25"/>
       <c r="C63" s="12" t="s">
         <v>29</v>
       </c>
@@ -2091,9 +2099,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15.75">
-      <c r="A64" s="25"/>
-      <c r="B64" s="24"/>
+    <row r="64" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="26"/>
+      <c r="B64" s="25"/>
       <c r="C64" s="12" t="s">
         <v>30</v>
       </c>
@@ -2108,9 +2116,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="15.75">
-      <c r="A65" s="25"/>
-      <c r="B65" s="24"/>
+    <row r="65" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="26"/>
+      <c r="B65" s="25"/>
       <c r="C65" s="12" t="s">
         <v>25</v>
       </c>
@@ -2124,11 +2132,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="15.75">
-      <c r="A66" s="25">
+    <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="26">
         <v>4</v>
       </c>
-      <c r="B66" s="24" t="s">
+      <c r="B66" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C66" s="12" t="s">
@@ -2144,9 +2152,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="15.75">
-      <c r="A67" s="25"/>
-      <c r="B67" s="24"/>
+    <row r="67" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="26"/>
+      <c r="B67" s="25"/>
       <c r="C67" s="12" t="s">
         <v>34</v>
       </c>
@@ -2162,9 +2170,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15.75">
-      <c r="A68" s="25"/>
-      <c r="B68" s="24"/>
+    <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="26"/>
+      <c r="B68" s="25"/>
       <c r="C68" s="12" t="s">
         <v>16</v>
       </c>
@@ -2178,9 +2186,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15.75">
-      <c r="A69" s="25"/>
-      <c r="B69" s="24"/>
+    <row r="69" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="26"/>
+      <c r="B69" s="25"/>
       <c r="C69" s="10" t="s">
         <v>31</v>
       </c>
@@ -2190,9 +2198,9 @@
       <c r="G69" s="19"/>
       <c r="H69" s="18"/>
     </row>
-    <row r="70" spans="1:8" ht="15.75">
-      <c r="A70" s="25"/>
-      <c r="B70" s="24"/>
+    <row r="70" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="26"/>
+      <c r="B70" s="25"/>
       <c r="C70" s="11" t="s">
         <v>33</v>
       </c>
@@ -2212,9 +2220,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15.75">
-      <c r="A71" s="25"/>
-      <c r="B71" s="24"/>
+    <row r="71" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="26"/>
+      <c r="B71" s="25"/>
       <c r="C71" s="11" t="s">
         <v>32</v>
       </c>
@@ -2234,9 +2242,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15.75">
-      <c r="A72" s="25"/>
-      <c r="B72" s="24"/>
+    <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="26"/>
+      <c r="B72" s="25"/>
       <c r="C72" s="12" t="s">
         <v>35</v>
       </c>
@@ -2256,9 +2264,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15.75">
-      <c r="A73" s="25"/>
-      <c r="B73" s="24"/>
+    <row r="73" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="26"/>
+      <c r="B73" s="25"/>
       <c r="C73" s="13" t="s">
         <v>36</v>
       </c>
@@ -2278,9 +2286,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15.75">
-      <c r="A74" s="25"/>
-      <c r="B74" s="24"/>
+    <row r="74" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="26"/>
+      <c r="B74" s="25"/>
       <c r="C74" s="13" t="s">
         <v>25</v>
       </c>
@@ -2294,11 +2302,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15.75">
-      <c r="A75" s="21">
+    <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="22">
         <v>5</v>
       </c>
-      <c r="B75" s="24" t="s">
+      <c r="B75" s="25" t="s">
         <v>17</v>
       </c>
       <c r="C75" s="5" t="s">
@@ -2314,9 +2322,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15.75">
-      <c r="A76" s="21"/>
-      <c r="B76" s="24"/>
+    <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="22"/>
+      <c r="B76" s="25"/>
       <c r="C76" s="5" t="s">
         <v>38</v>
       </c>
@@ -2330,9 +2338,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15.75">
-      <c r="A77" s="21"/>
-      <c r="B77" s="24"/>
+    <row r="77" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="22"/>
+      <c r="B77" s="25"/>
       <c r="C77" s="5" t="s">
         <v>39</v>
       </c>
@@ -2346,9 +2354,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15.75">
-      <c r="A78" s="21"/>
-      <c r="B78" s="24"/>
+    <row r="78" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="22"/>
+      <c r="B78" s="25"/>
       <c r="C78" s="14" t="s">
         <v>25</v>
       </c>
@@ -2362,11 +2370,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15.75">
-      <c r="A79" s="21">
+    <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="22">
         <v>6</v>
       </c>
-      <c r="B79" s="24" t="s">
+      <c r="B79" s="25" t="s">
         <v>7</v>
       </c>
       <c r="C79" s="13" t="s">
@@ -2382,9 +2390,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15.75">
-      <c r="A80" s="21"/>
-      <c r="B80" s="24"/>
+    <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="22"/>
+      <c r="B80" s="25"/>
       <c r="C80" s="13" t="s">
         <v>15</v>
       </c>
@@ -2398,9 +2406,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15.75">
-      <c r="A81" s="21"/>
-      <c r="B81" s="24"/>
+    <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="22"/>
+      <c r="B81" s="25"/>
       <c r="C81" s="13" t="s">
         <v>25</v>
       </c>
@@ -2414,11 +2422,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15.75">
-      <c r="A82" s="21">
+    <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="22">
         <v>7</v>
       </c>
-      <c r="B82" s="26" t="s">
+      <c r="B82" s="21" t="s">
         <v>40</v>
       </c>
       <c r="C82" s="5" t="s">
@@ -2440,9 +2448,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.75">
-      <c r="A83" s="21"/>
-      <c r="B83" s="26"/>
+    <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="22"/>
+      <c r="B83" s="21"/>
       <c r="C83" s="5" t="s">
         <v>46</v>
       </c>
@@ -2462,11 +2470,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15.75">
-      <c r="A84" s="21">
-        <v>8</v>
-      </c>
-      <c r="B84" s="26" t="s">
+    <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="22">
+        <v>8</v>
+      </c>
+      <c r="B84" s="21" t="s">
         <v>42</v>
       </c>
       <c r="C84" s="5" t="s">
@@ -2482,9 +2490,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="15.75">
-      <c r="A85" s="21"/>
-      <c r="B85" s="26"/>
+    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="22"/>
+      <c r="B85" s="21"/>
       <c r="C85" s="14" t="s">
         <v>43</v>
       </c>
@@ -2500,11 +2508,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="15.75">
-      <c r="A86" s="22">
+    <row r="86" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="23">
         <v>9</v>
       </c>
-      <c r="B86" s="23" t="s">
+      <c r="B86" s="24" t="s">
         <v>49</v>
       </c>
       <c r="C86" s="14" t="s">
@@ -2522,9 +2530,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="15.75">
-      <c r="A87" s="22"/>
-      <c r="B87" s="23"/>
+    <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="23"/>
+      <c r="B87" s="24"/>
       <c r="C87" s="14" t="s">
         <v>97</v>
       </c>
@@ -2537,12 +2545,12 @@
         <v>8</v>
       </c>
       <c r="H87" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="15.75">
-      <c r="A88" s="22"/>
-      <c r="B88" s="23"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="23"/>
+      <c r="B88" s="24"/>
       <c r="C88" s="14" t="s">
         <v>98</v>
       </c>
@@ -2556,9 +2564,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15.75">
-      <c r="A89" s="22"/>
-      <c r="B89" s="23"/>
+    <row r="89" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="23"/>
+      <c r="B89" s="24"/>
       <c r="C89" s="14" t="s">
         <v>99</v>
       </c>
@@ -2569,12 +2577,12 @@
       <c r="F89" s="16"/>
       <c r="G89" s="16"/>
       <c r="H89" s="17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="15.75">
-      <c r="A90" s="22"/>
-      <c r="B90" s="23"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="23"/>
+      <c r="B90" s="24"/>
       <c r="C90" s="14" t="s">
         <v>100</v>
       </c>
@@ -2589,12 +2597,12 @@
         <v>8</v>
       </c>
       <c r="H90" s="17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="15.75">
-      <c r="A91" s="22"/>
-      <c r="B91" s="23"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="23"/>
+      <c r="B91" s="24"/>
       <c r="C91" s="14" t="s">
         <v>48</v>
       </c>
@@ -2605,39 +2613,29 @@
         <v>8</v>
       </c>
       <c r="H91" s="17">
-        <v>15</v>
-      </c>
-      <c r="I91">
-        <f>SUM(H86:H91)</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="H92">
-        <f>SUM(H2:H91)</f>
-        <v>163</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="B66:B74"/>
+    <mergeCell ref="A66:A74"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B15:B65"/>
+    <mergeCell ref="A15:A65"/>
+    <mergeCell ref="A10:A14"/>
     <mergeCell ref="B82:B83"/>
     <mergeCell ref="B84:B85"/>
     <mergeCell ref="A82:A83"/>
     <mergeCell ref="A84:A85"/>
     <mergeCell ref="A86:A91"/>
     <mergeCell ref="B86:B91"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B15:B65"/>
-    <mergeCell ref="A15:A65"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="B66:B74"/>
-    <mergeCell ref="A66:A74"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <dataValidations count="1">
@@ -2657,7 +2655,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2669,7 +2667,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>